<commit_message>
Added Steve's user stories
</commit_message>
<xml_diff>
--- a/Proposals/UserStories.xlsx
+++ b/Proposals/UserStories.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\GitHub\2016Elections\Proposals\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Users\johno_000\Documents\GitHub\2016Elections\Proposals\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t>Use Case</t>
   </si>
@@ -99,6 +99,45 @@
   </si>
   <si>
     <t>John</t>
+  </si>
+  <si>
+    <t>Administrator</t>
+  </si>
+  <si>
+    <t>Designate points on map that link with stories.</t>
+  </si>
+  <si>
+    <t>To provide users an easy way to view the location to which a story is connected.</t>
+  </si>
+  <si>
+    <t>A story has been posted.</t>
+  </si>
+  <si>
+    <t>A point on the map is linked with the story.</t>
+  </si>
+  <si>
+    <t>Delete or edit submissions by users and content publishers.</t>
+  </si>
+  <si>
+    <t>To provide the ability to moderate posts and comments in case inappropriate content is submitted.</t>
+  </si>
+  <si>
+    <t>A post/comment has been submitted and an administrator has a reason to edit or delete it.</t>
+  </si>
+  <si>
+    <t>The post/comment has been changed or deleted.</t>
+  </si>
+  <si>
+    <t>View analytics about the website such as demographics and page views</t>
+  </si>
+  <si>
+    <t>To give administrators meaningful statistics about the website.</t>
+  </si>
+  <si>
+    <t>Analytics have been collected and administrator is logged in.</t>
+  </si>
+  <si>
+    <t>The administrator is able to view analytics.</t>
   </si>
 </sst>
 </file>
@@ -422,7 +461,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,28 +565,73 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
       <c r="B10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated User stories excel
</commit_message>
<xml_diff>
--- a/Proposals/UserStories.xlsx
+++ b/Proposals/UserStories.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Users\johno_000\Documents\GitHub\2016Elections\Proposals\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\GitHub\2016Elections\Proposals\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
   <si>
     <t>Use Case</t>
   </si>
@@ -138,6 +138,54 @@
   </si>
   <si>
     <t>The administrator is able to view analytics.</t>
+  </si>
+  <si>
+    <t>Create a new topic</t>
+  </si>
+  <si>
+    <t>To provide a forum for users to post in</t>
+  </si>
+  <si>
+    <t>There is not an identical forum topic</t>
+  </si>
+  <si>
+    <t>Users can post content inside of the topic</t>
+  </si>
+  <si>
+    <t>To see content that other users have posted</t>
+  </si>
+  <si>
+    <t>Content has been posted</t>
+  </si>
+  <si>
+    <t>Users can respond to post, Administrator can edit and delete posts</t>
+  </si>
+  <si>
+    <t>Allows user to create their own personal account</t>
+  </si>
+  <si>
+    <t>To allow users to join and contribute to the community</t>
+  </si>
+  <si>
+    <t>User does not have an account</t>
+  </si>
+  <si>
+    <t>User now has access to privilege given to their user class</t>
+  </si>
+  <si>
+    <t>Administrator, Content Publisher, Registered User, Unregistered User</t>
+  </si>
+  <si>
+    <t>Unregistered User</t>
+  </si>
+  <si>
+    <t>Allow all users to view content posted</t>
+  </si>
+  <si>
+    <t>Possible Breakdown?</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -458,23 +506,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
     <col min="5" max="5" width="23.5703125" customWidth="1"/>
     <col min="6" max="6" width="29.85546875" customWidth="1"/>
     <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -493,8 +542,11 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -517,23 +569,29 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -541,31 +599,76 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -588,7 +691,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -611,7 +714,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Added requirement proposal pdf, updated user case diagrams
Updated all user stories with submissions and uploaded a quick .pdf for
standard viewing
</commit_message>
<xml_diff>
--- a/Proposals/UserStories.xlsx
+++ b/Proposals/UserStories.xlsx
@@ -506,24 +506,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
     <col min="5" max="5" width="23.5703125" customWidth="1"/>
     <col min="6" max="6" width="29.85546875" customWidth="1"/>
     <col min="7" max="7" width="17.5703125" customWidth="1"/>
     <col min="8" max="8" width="21.85546875" customWidth="1"/>
+    <col min="9" max="9" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -546,7 +547,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -568,8 +569,17 @@
       <c r="G2" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="1" t="str">
+        <f>ROW()-1&amp;". "&amp;B2&amp;CHAR(10)&amp;$C$1&amp;": "&amp;C2&amp;CHAR(10)&amp;$D$1&amp;": "&amp;D2&amp;CHAR(10)&amp;$E$1&amp;": "&amp;E2&amp;CHAR(10)&amp;$F$1&amp;": "&amp;F2&amp;CHAR(10)&amp;$G$1&amp;": "&amp;G2</f>
+        <v>1. Post Content Link
+User Role: Content Publisher
+Goal: To post a link to an article hosted on a 3rd party website.
+Reason: To provide users with content relevant to the elections and local news.
+Pre-Conditions: Content publisher is logged in, an article has been found, and a link is available to the content. 
+Post-Conditions: The link is posted to the website and available for users to view.</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -579,8 +589,17 @@
       <c r="H3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="1" t="str">
+        <f t="shared" ref="I3:I12" si="0">ROW()-1&amp;". "&amp;B3&amp;CHAR(10)&amp;$C$1&amp;": "&amp;C3&amp;CHAR(10)&amp;$D$1&amp;": "&amp;D3&amp;CHAR(10)&amp;$E$1&amp;": "&amp;E3&amp;CHAR(10)&amp;$F$1&amp;": "&amp;F3&amp;CHAR(10)&amp;$G$1&amp;": "&amp;G3</f>
+        <v xml:space="preserve">2. Post Content
+User Role: 
+Goal: 
+Reason: 
+Pre-Conditions: 
+Post-Conditions: </v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -590,16 +609,34 @@
       <c r="H4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">3. Update Live Coverage
+User Role: 
+Goal: 
+Reason: 
+Pre-Conditions: 
+Post-Conditions: </v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">4. Post in Forum/Comment
+User Role: 
+Goal: 
+Reason: 
+Pre-Conditions: 
+Post-Conditions: </v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -621,8 +658,17 @@
       <c r="G6" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="I6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>5. Create Forum Topic
+User Role: Administrator
+Goal: Create a new topic
+Reason: To provide a forum for users to post in
+Pre-Conditions: There is not an identical forum topic
+Post-Conditions: Users can post content inside of the topic</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -644,8 +690,17 @@
       <c r="G7" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="I7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>6. View Content
+User Role: Administrator, Content Publisher, Registered User, Unregistered User
+Goal: Allow all users to view content posted
+Reason: To see content that other users have posted
+Pre-Conditions: Content has been posted
+Post-Conditions: Users can respond to post, Administrator can edit and delete posts</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -667,8 +722,17 @@
       <c r="G8" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="I8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>7. Create Account
+User Role: Unregistered User
+Goal: Allows user to create their own personal account
+Reason: To allow users to join and contribute to the community
+Pre-Conditions: User does not have an account
+Post-Conditions: User now has access to privilege given to their user class</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -690,8 +754,17 @@
       <c r="G9" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="I9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>8. Update Map Data
+User Role: Administrator
+Goal: Designate points on map that link with stories.
+Reason: To provide users an easy way to view the location to which a story is connected.
+Pre-Conditions: A story has been posted.
+Post-Conditions: A point on the map is linked with the story.</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -713,8 +786,17 @@
       <c r="G10" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="I10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>9. Delete or Edit Post/Comment
+User Role: Administrator
+Goal: Delete or edit submissions by users and content publishers.
+Reason: To provide the ability to moderate posts and comments in case inappropriate content is submitted.
+Pre-Conditions: A post/comment has been submitted and an administrator has a reason to edit or delete it.
+Post-Conditions: The post/comment has been changed or deleted.</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -735,6 +817,26 @@
       </c>
       <c r="G11" s="1" t="s">
         <v>37</v>
+      </c>
+      <c r="I11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>10. View Analytics
+User Role: Administrator
+Goal: View analytics about the website such as demographics and page views
+Reason: To give administrators meaningful statistics about the website.
+Pre-Conditions: Analytics have been collected and administrator is logged in.
+Post-Conditions: The administrator is able to view analytics.</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="I12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">11. 
+User Role: 
+Goal: 
+Reason: 
+Pre-Conditions: 
+Post-Conditions: </v>
       </c>
     </row>
   </sheetData>

</xml_diff>